<commit_message>
Improve formatting of seating plan excel
</commit_message>
<xml_diff>
--- a/uploads/test_file.xlsx
+++ b/uploads/test_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ea64feece74fddb/Desktop/SWDC EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_A28C42611EE90B0163A5D04BF120EF0DB3C24D98" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{604E25AD-8F36-4966-9752-B07DAFB944BC}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="11_A28C42611EE90B0163A5D04BF120EF0DB3C24D98" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64A39313-C23F-40E7-9535-A423BC5E7690}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,9 +70,6 @@
     <t>SY</t>
   </si>
   <si>
-    <t>Comps</t>
-  </si>
-  <si>
     <t>DDL</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>DS</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
     <t>TY</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>J</t>
   </si>
   <si>
-    <t>ITVC</t>
-  </si>
-  <si>
     <t>COA</t>
   </si>
   <si>
@@ -158,6 +149,15 @@
   </si>
   <si>
     <t>TACD</t>
+  </si>
+  <si>
+    <t>B.Tech COMP</t>
+  </si>
+  <si>
+    <t>B.Tech ITVC</t>
+  </si>
+  <si>
+    <t>B.Tech IT</t>
   </si>
 </sst>
 </file>
@@ -229,6 +229,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -585,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -594,19 +598,19 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -614,7 +618,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -623,19 +627,19 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -643,7 +647,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -652,19 +656,19 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -672,7 +676,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -681,19 +685,19 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -701,7 +705,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -710,19 +714,19 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -730,7 +734,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -739,27 +743,27 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2">
         <v>5</v>
@@ -768,27 +772,27 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2">
         <v>5</v>
@@ -797,27 +801,27 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
@@ -826,27 +830,27 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2">
         <v>5</v>
@@ -855,19 +859,19 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
         <v>37</v>
       </c>
-      <c r="G11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" t="s">
-        <v>40</v>
-      </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -875,7 +879,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
@@ -884,19 +888,19 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -904,7 +908,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
@@ -913,19 +917,19 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -933,7 +937,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
@@ -942,19 +946,19 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -962,7 +966,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2">
         <v>3</v>
@@ -971,19 +975,19 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -991,7 +995,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2">
         <v>4</v>
@@ -1000,19 +1004,19 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1020,7 +1024,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2">
         <v>4</v>
@@ -1029,27 +1033,27 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" t="s">
         <v>18</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2">
         <v>5</v>
@@ -1058,27 +1062,27 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2">
         <v>5</v>
@@ -1087,27 +1091,27 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2">
         <v>5</v>
@@ -1116,27 +1120,27 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2">
         <v>5</v>
@@ -1145,19 +1149,19 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
         <v>37</v>
       </c>
-      <c r="G21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" t="s">
-        <v>40</v>
-      </c>
       <c r="I21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1165,7 +1169,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C22" s="2">
         <v>3</v>
@@ -1174,19 +1178,19 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1194,28 +1198,28 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="2">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" t="s">
-        <v>17</v>
-      </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1223,7 +1227,7 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2">
         <v>3</v>
@@ -1232,19 +1236,19 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1252,7 +1256,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C25" s="2">
         <v>3</v>
@@ -1261,19 +1265,19 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1281,7 +1285,7 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C26" s="2">
         <v>4</v>
@@ -1290,19 +1294,19 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1310,7 +1314,7 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C27" s="2">
         <v>4</v>
@@ -1319,27 +1323,27 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" t="s">
         <v>18</v>
-      </c>
-      <c r="G27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2">
         <v>5</v>
@@ -1348,27 +1352,27 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C29" s="2">
         <v>5</v>
@@ -1377,27 +1381,27 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C30" s="2">
         <v>5</v>
@@ -1406,27 +1410,27 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C31" s="2">
         <v>5</v>
@@ -1435,19 +1439,19 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" t="s">
         <v>37</v>
       </c>
-      <c r="G31" t="s">
-        <v>38</v>
-      </c>
-      <c r="H31" t="s">
-        <v>40</v>
-      </c>
       <c r="I31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1455,7 +1459,7 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C32" s="2">
         <v>3</v>
@@ -1464,19 +1468,19 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1484,7 +1488,7 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2">
         <v>3</v>
@@ -1493,19 +1497,19 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1513,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C34" s="2">
         <v>3</v>
@@ -1522,19 +1526,19 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1542,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2">
         <v>3</v>
@@ -1551,19 +1555,19 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1571,7 +1575,7 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C36" s="2">
         <v>4</v>
@@ -1580,19 +1584,19 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1600,7 +1604,7 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C37" s="2">
         <v>4</v>
@@ -1609,27 +1613,27 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" t="s">
         <v>18</v>
-      </c>
-      <c r="G37" t="s">
-        <v>45</v>
-      </c>
-      <c r="H37" t="s">
-        <v>21</v>
-      </c>
-      <c r="I37" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C38" s="2">
         <v>5</v>
@@ -1638,27 +1642,27 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H38" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C39" s="2">
         <v>5</v>
@@ -1667,27 +1671,27 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I39" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C40" s="2">
         <v>5</v>
@@ -1696,27 +1700,27 @@
         <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G40" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I40" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2">
         <v>5</v>
@@ -1725,19 +1729,19 @@
         <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" t="s">
         <v>37</v>
       </c>
-      <c r="G41" t="s">
-        <v>38</v>
-      </c>
-      <c r="H41" t="s">
-        <v>40</v>
-      </c>
       <c r="I41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1745,7 +1749,7 @@
         <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C42" s="2">
         <v>3</v>
@@ -1754,19 +1758,19 @@
         <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G42" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I42" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1774,7 +1778,7 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C43" s="2">
         <v>3</v>
@@ -1783,19 +1787,19 @@
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F43" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1803,7 +1807,7 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C44" s="2">
         <v>3</v>
@@ -1812,19 +1816,19 @@
         <v>43</v>
       </c>
       <c r="E44" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G44" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I44" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1832,7 +1836,7 @@
         <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C45" s="2">
         <v>3</v>
@@ -1841,19 +1845,19 @@
         <v>44</v>
       </c>
       <c r="E45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H45" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I45" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1861,7 +1865,7 @@
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C46" s="2">
         <v>4</v>
@@ -1870,19 +1874,19 @@
         <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1890,7 +1894,7 @@
         <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C47" s="2">
         <v>4</v>
@@ -1899,27 +1903,27 @@
         <v>46</v>
       </c>
       <c r="E47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F47" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" t="s">
+        <v>42</v>
+      </c>
+      <c r="H47" t="s">
+        <v>20</v>
+      </c>
+      <c r="I47" t="s">
         <v>18</v>
-      </c>
-      <c r="G47" t="s">
-        <v>45</v>
-      </c>
-      <c r="H47" t="s">
-        <v>21</v>
-      </c>
-      <c r="I47" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C48" s="2">
         <v>5</v>
@@ -1928,27 +1932,27 @@
         <v>47</v>
       </c>
       <c r="E48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H48" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I48" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C49" s="2">
         <v>5</v>
@@ -1957,27 +1961,27 @@
         <v>48</v>
       </c>
       <c r="E49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F49" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I49" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C50" s="2">
         <v>5</v>
@@ -1986,27 +1990,27 @@
         <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F50" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G50" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C51" s="2">
         <v>5</v>
@@ -2015,19 +2019,19 @@
         <v>50</v>
       </c>
       <c r="E51" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F51" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" t="s">
+        <v>35</v>
+      </c>
+      <c r="H51" t="s">
         <v>37</v>
       </c>
-      <c r="G51" t="s">
-        <v>38</v>
-      </c>
-      <c r="H51" t="s">
-        <v>40</v>
-      </c>
       <c r="I51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2035,7 +2039,7 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C52" s="2">
         <v>3</v>
@@ -2044,19 +2048,19 @@
         <v>51</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G52" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H52" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I52" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2064,7 +2068,7 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C53" s="2">
         <v>3</v>
@@ -2073,19 +2077,19 @@
         <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F53" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H53" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I53" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2093,7 +2097,7 @@
         <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C54" s="2">
         <v>3</v>
@@ -2102,19 +2106,19 @@
         <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G54" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H54" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I54" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,7 +2126,7 @@
         <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C55" s="2">
         <v>3</v>
@@ -2131,19 +2135,19 @@
         <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H55" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2151,7 +2155,7 @@
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C56" s="2">
         <v>4</v>
@@ -2160,19 +2164,19 @@
         <v>55</v>
       </c>
       <c r="E56" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2180,7 +2184,7 @@
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C57" s="2">
         <v>4</v>
@@ -2189,27 +2193,27 @@
         <v>56</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F57" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" t="s">
+        <v>42</v>
+      </c>
+      <c r="H57" t="s">
+        <v>20</v>
+      </c>
+      <c r="I57" t="s">
         <v>18</v>
-      </c>
-      <c r="G57" t="s">
-        <v>45</v>
-      </c>
-      <c r="H57" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C58" s="2">
         <v>5</v>
@@ -2218,27 +2222,27 @@
         <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G58" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H58" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I58" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C59" s="2">
         <v>5</v>
@@ -2247,27 +2251,27 @@
         <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F59" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H59" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I59" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C60" s="2">
         <v>5</v>
@@ -2276,27 +2280,27 @@
         <v>59</v>
       </c>
       <c r="E60" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F60" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G60" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I60" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C61" s="2">
         <v>5</v>
@@ -2305,19 +2309,19 @@
         <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F61" t="s">
+        <v>34</v>
+      </c>
+      <c r="G61" t="s">
+        <v>35</v>
+      </c>
+      <c r="H61" t="s">
         <v>37</v>
       </c>
-      <c r="G61" t="s">
-        <v>38</v>
-      </c>
-      <c r="H61" t="s">
-        <v>40</v>
-      </c>
       <c r="I61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2325,7 +2329,7 @@
         <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C62" s="2">
         <v>3</v>
@@ -2334,19 +2338,19 @@
         <v>61</v>
       </c>
       <c r="E62" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G62" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H62" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I62" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2354,7 +2358,7 @@
         <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C63" s="2">
         <v>3</v>
@@ -2363,19 +2367,19 @@
         <v>62</v>
       </c>
       <c r="E63" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H63" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I63" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2383,7 +2387,7 @@
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C64" s="2">
         <v>3</v>
@@ -2392,19 +2396,19 @@
         <v>63</v>
       </c>
       <c r="E64" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G64" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H64" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I64" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2412,7 +2416,7 @@
         <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C65" s="2">
         <v>3</v>
@@ -2421,19 +2425,19 @@
         <v>64</v>
       </c>
       <c r="E65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F65" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H65" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I65" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2441,7 +2445,7 @@
         <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C66" s="2">
         <v>4</v>
@@ -2450,19 +2454,19 @@
         <v>65</v>
       </c>
       <c r="E66" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F66" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2470,7 +2474,7 @@
         <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C67" s="2">
         <v>4</v>
@@ -2479,27 +2483,27 @@
         <v>66</v>
       </c>
       <c r="E67" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F67" t="s">
+        <v>17</v>
+      </c>
+      <c r="G67" t="s">
+        <v>42</v>
+      </c>
+      <c r="H67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I67" t="s">
         <v>18</v>
-      </c>
-      <c r="G67" t="s">
-        <v>45</v>
-      </c>
-      <c r="H67" t="s">
-        <v>21</v>
-      </c>
-      <c r="I67" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C68" s="2">
         <v>5</v>
@@ -2508,27 +2512,27 @@
         <v>67</v>
       </c>
       <c r="E68" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G68" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I68" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B69" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C69" s="2">
         <v>5</v>
@@ -2537,27 +2541,27 @@
         <v>68</v>
       </c>
       <c r="E69" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F69" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H69" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C70" s="2">
         <v>5</v>
@@ -2566,27 +2570,27 @@
         <v>69</v>
       </c>
       <c r="E70" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F70" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G70" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I70" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C71" s="2">
         <v>5</v>
@@ -2595,19 +2599,19 @@
         <v>70</v>
       </c>
       <c r="E71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F71" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71" t="s">
+        <v>35</v>
+      </c>
+      <c r="H71" t="s">
         <v>37</v>
       </c>
-      <c r="G71" t="s">
-        <v>38</v>
-      </c>
-      <c r="H71" t="s">
-        <v>40</v>
-      </c>
       <c r="I71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2615,7 +2619,7 @@
         <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C72" s="2">
         <v>3</v>
@@ -2624,19 +2628,19 @@
         <v>71</v>
       </c>
       <c r="E72" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G72" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H72" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I72" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2644,7 +2648,7 @@
         <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C73" s="2">
         <v>3</v>
@@ -2653,19 +2657,19 @@
         <v>72</v>
       </c>
       <c r="E73" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F73" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H73" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I73" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2673,7 +2677,7 @@
         <v>15</v>
       </c>
       <c r="B74" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C74" s="2">
         <v>3</v>
@@ -2682,19 +2686,19 @@
         <v>73</v>
       </c>
       <c r="E74" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G74" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H74" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I74" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2702,7 +2706,7 @@
         <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C75" s="2">
         <v>3</v>
@@ -2711,19 +2715,19 @@
         <v>74</v>
       </c>
       <c r="E75" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F75" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H75" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I75" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2731,7 +2735,7 @@
         <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C76" s="2">
         <v>4</v>
@@ -2740,19 +2744,19 @@
         <v>75</v>
       </c>
       <c r="E76" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F76" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H76" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2760,7 +2764,7 @@
         <v>15</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C77" s="2">
         <v>4</v>
@@ -2769,27 +2773,27 @@
         <v>76</v>
       </c>
       <c r="E77" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F77" t="s">
+        <v>17</v>
+      </c>
+      <c r="G77" t="s">
+        <v>42</v>
+      </c>
+      <c r="H77" t="s">
+        <v>20</v>
+      </c>
+      <c r="I77" t="s">
         <v>18</v>
-      </c>
-      <c r="G77" t="s">
-        <v>45</v>
-      </c>
-      <c r="H77" t="s">
-        <v>21</v>
-      </c>
-      <c r="I77" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C78" s="2">
         <v>5</v>
@@ -2798,27 +2802,27 @@
         <v>77</v>
       </c>
       <c r="E78" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G78" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H78" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I78" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C79" s="2">
         <v>5</v>
@@ -2827,27 +2831,27 @@
         <v>78</v>
       </c>
       <c r="E79" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F79" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H79" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I79" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C80" s="2">
         <v>5</v>
@@ -2856,27 +2860,27 @@
         <v>79</v>
       </c>
       <c r="E80" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F80" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G80" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H80" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I80" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C81" s="2">
         <v>5</v>
@@ -2885,19 +2889,19 @@
         <v>80</v>
       </c>
       <c r="E81" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F81" t="s">
+        <v>34</v>
+      </c>
+      <c r="G81" t="s">
+        <v>35</v>
+      </c>
+      <c r="H81" t="s">
         <v>37</v>
       </c>
-      <c r="G81" t="s">
-        <v>38</v>
-      </c>
-      <c r="H81" t="s">
-        <v>40</v>
-      </c>
       <c r="I81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>